<commit_message>
Added log4j dependencies, created log4j2 xml file, log4j utility class, Testlistener class and created necessary loggers for different classes.
</commit_message>
<xml_diff>
--- a/testData/loginData.xlsx
+++ b/testData/loginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/214e555ca58eeef7/Desktop/Eclipse workspaces/proj1/automationAssignment/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_F25DC773A252ABDACC104861611E5B205ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7F3FB4B-C11C-4D9B-BD0F-1072740F116A}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_F25DC773A252ABDACC104861611E5B205ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B96970A4-B6B9-40A1-89B3-9E1DD7CBC473}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>emailAddress</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>Pass1234</t>
-  </si>
-  <si>
-    <t>abc@gmail.com</t>
   </si>
   <si>
     <t>solih48913@gamebcs.com</t>
@@ -95,6 +92,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -360,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -396,14 +397,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added 2 new tests in the framework.
</commit_message>
<xml_diff>
--- a/testData/loginData.xlsx
+++ b/testData/loginData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/214e555ca58eeef7/Desktop/Eclipse workspaces/proj1/automationAssignment/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_F25DC773A252ABDACC104861611E5B205ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B96970A4-B6B9-40A1-89B3-9E1DD7CBC473}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_F25DC773A252ABDACC104861611E5B205ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8016CDB-5D2D-463B-9C17-765115601CDF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>emailAddress</t>
   </si>
   <si>
     <t>password</t>
-  </si>
-  <si>
-    <t>shardulpakhare@gmail.com</t>
   </si>
   <si>
     <t>Pass1234</t>
@@ -361,10 +358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -383,18 +380,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>